<commit_message>
updated admin/Menu.xlsx (changed uuid)
</commit_message>
<xml_diff>
--- a/admin/Menu.xlsx
+++ b/admin/Menu.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Александр\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dmitrii\PycharmProjects\FastAPI_Restaurant\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{166AE2FF-4742-4057-ACD4-10D4DB500A86}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Меню</t>
   </si>
@@ -132,12 +133,66 @@
   </si>
   <si>
     <t>Нарезка из ветчины, колбасных колечек, нескольких сортов сыра и фруктов</t>
+  </si>
+  <si>
+    <t>c2ddea44-b60b-49ad-b919-7e40ecddcdb9</t>
+  </si>
+  <si>
+    <t>08f8c612-2700-406e-88df-eae964a98f67</t>
+  </si>
+  <si>
+    <t>7cbb7091-747e-4d5c-82e5-d7da589888e9</t>
+  </si>
+  <si>
+    <t>59c4f253-c906-4e42-a81d-75a735e299ef</t>
+  </si>
+  <si>
+    <t>2f14b53d-1bcc-4a1b-97ca-d08cfedbc31c</t>
+  </si>
+  <si>
+    <t>5b0a804a-d0c0-45c7-9ef0-bf5a5bba271a</t>
+  </si>
+  <si>
+    <t>7580d708-5314-4212-a30d-81fad3738b59</t>
+  </si>
+  <si>
+    <t>29a5e408-08c7-4f66-9432-972dd4d644b3</t>
+  </si>
+  <si>
+    <t>2cde7d42-04a6-42ad-8d2d-7ed704185105</t>
+  </si>
+  <si>
+    <t>f48aab6b-64e7-4aa8-8b0e-f70c4afe8cec</t>
+  </si>
+  <si>
+    <t>b27a63ba-0104-4471-992a-a6503a940cd0</t>
+  </si>
+  <si>
+    <t>3117ee28-6d3f-4586-a027-7addd15d0c42</t>
+  </si>
+  <si>
+    <t>f1c96124-e005-467e-b2f6-86be90a8eb03</t>
+  </si>
+  <si>
+    <t>6e56c599-9fb4-47e6-b7cd-191e59634c7b</t>
+  </si>
+  <si>
+    <t>ee3fad65-2876-45c4-9e91-7ca21405df92</t>
+  </si>
+  <si>
+    <t>230daedc-6335-416f-95b4-ecfd952f60dc</t>
+  </si>
+  <si>
+    <t>2cc28716-4861-4ca0-b78e-aa9194c28e1f</t>
+  </si>
+  <si>
+    <t>c27fa7a9-1170-4224-b73d-eb1b9e8c58a8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2">
     <font>
       <sz val="10"/>
@@ -187,14 +242,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -422,29 +473,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F1000"/>
+  <dimension ref="A1:F999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" style="9" customWidth="1"/>
-    <col min="5" max="5" width="77.7109375" style="9" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="77.6640625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A1" s="1">
-        <v>1</v>
+      <c r="A1" t="s">
+        <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -452,96 +503,96 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="2"/>
-      <c r="B2" s="1">
-        <v>1</v>
+      <c r="B2" t="s">
+        <v>36</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="8"/>
+      <c r="E2" s="6"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="8" t="s">
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>182.99</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16.5" customHeight="1">
       <c r="A4" s="2"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="3">
-        <v>2</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>215.36</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="2"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="3">
-        <v>3</v>
-      </c>
-      <c r="D5" s="8" t="s">
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>265.57</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="A6" s="2"/>
-      <c r="B6" s="1">
-        <v>2</v>
+      <c r="B6" t="s">
+        <v>39</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="7"/>
+      <c r="E6" s="5"/>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="8" t="s">
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="1">
@@ -551,13 +602,13 @@
     <row r="8" spans="1:6" ht="15.75" customHeight="1">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="1">
-        <v>2</v>
-      </c>
-      <c r="D8" s="8" t="s">
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F8" s="1">
@@ -567,13 +618,13 @@
     <row r="9" spans="1:6" ht="15.75" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
-      <c r="C9" s="1">
-        <v>3</v>
-      </c>
-      <c r="D9" s="8" t="s">
+      <c r="C9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="5" t="s">
         <v>16</v>
       </c>
       <c r="F9" s="1">
@@ -581,8 +632,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A10" s="5">
-        <v>2</v>
+      <c r="A10" t="s">
+        <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>17</v>
@@ -590,34 +641,34 @@
       <c r="C10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="7"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="5"/>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1">
       <c r="A11" s="2"/>
-      <c r="B11" s="1">
-        <v>1</v>
+      <c r="B11" t="s">
+        <v>52</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="7"/>
+      <c r="E11" s="5"/>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1">
       <c r="A12" s="2"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="3">
-        <v>1</v>
-      </c>
-      <c r="D12" s="8" t="s">
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F12" s="1">
@@ -627,13 +678,13 @@
     <row r="13" spans="1:6" ht="15.75" customHeight="1">
       <c r="A13" s="2"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="3">
-        <v>2</v>
-      </c>
-      <c r="D13" s="8" t="s">
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="5" t="s">
         <v>24</v>
       </c>
       <c r="F13" s="1">
@@ -643,13 +694,13 @@
     <row r="14" spans="1:6" ht="15.75" customHeight="1">
       <c r="A14" s="2"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="3">
-        <v>3</v>
-      </c>
-      <c r="D14" s="8" t="s">
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="5" t="s">
         <v>26</v>
       </c>
       <c r="F14" s="1">
@@ -658,28 +709,28 @@
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1">
       <c r="A15" s="2"/>
-      <c r="B15" s="1">
-        <v>2</v>
+      <c r="B15" t="s">
+        <v>53</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="7"/>
+      <c r="E15" s="5"/>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="1">
-        <v>1</v>
-      </c>
-      <c r="D16" s="8" t="s">
+      <c r="C16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="5" t="s">
         <v>30</v>
       </c>
       <c r="F16" s="1">
@@ -689,13 +740,13 @@
     <row r="17" spans="1:6" ht="15.75" customHeight="1">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="1">
-        <v>2</v>
-      </c>
-      <c r="D17" s="8" t="s">
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="5" t="s">
         <v>32</v>
       </c>
       <c r="F17" s="1">
@@ -705,13 +756,13 @@
     <row r="18" spans="1:6" ht="15.75" customHeight="1">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
-      <c r="C18" s="1">
-        <v>3</v>
-      </c>
-      <c r="D18" s="8" t="s">
+      <c r="C18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="5" t="s">
         <v>34</v>
       </c>
       <c r="F18" s="1">
@@ -1699,7 +1750,6 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated admin/Menu.xlxs (added percentage)
</commit_message>
<xml_diff>
--- a/admin/Menu.xlsx
+++ b/admin/Menu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dmitrii\PycharmProjects\FastAPI_Restaurant\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E92534-C0FB-4F8B-9ACD-D887F076D6E8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37A1692-C4AE-478C-9B3D-5A331E2480C2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -215,7 +215,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -238,15 +238,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -259,6 +286,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -477,10 +508,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F999"/>
+  <dimension ref="A1:G999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="A1:F18"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
@@ -488,12 +519,12 @@
     <col min="1" max="1" width="7.44140625" customWidth="1"/>
     <col min="2" max="2" width="20.88671875" customWidth="1"/>
     <col min="3" max="3" width="20.109375" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="77.6640625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="77.6640625" style="6" customWidth="1"/>
     <col min="6" max="6" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -503,11 +534,12 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="2"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="9"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" t="s">
         <v>36</v>
@@ -515,61 +547,71 @@
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="2"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="1"/>
       <c r="C3" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="8">
         <v>182.99</v>
       </c>
+      <c r="G3" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" ht="16.5" customHeight="1">
+    <row r="4" spans="1:7" ht="16.5" customHeight="1">
       <c r="A4" s="2"/>
       <c r="B4" s="1"/>
       <c r="C4" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="8">
         <v>215.36</v>
       </c>
+      <c r="G4" s="10">
+        <v>25</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1">
       <c r="A5" s="2"/>
       <c r="B5" s="1"/>
       <c r="C5" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="8">
         <v>265.57</v>
       </c>
+      <c r="G5" s="10">
+        <v>31</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
         <v>39</v>
@@ -577,61 +619,71 @@
       <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="2"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="7">
         <v>166.47</v>
       </c>
+      <c r="G7" s="10">
+        <v>25.5</v>
+      </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="7">
         <v>168.25</v>
       </c>
+      <c r="G8" s="10">
+        <v>73</v>
+      </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="7">
         <v>132.88</v>
       </c>
+      <c r="G9" s="10">
+        <v>99.99</v>
+      </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -641,11 +693,12 @@
       <c r="C10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="2"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="10"/>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
       <c r="A11" s="2"/>
       <c r="B11" t="s">
         <v>52</v>
@@ -653,61 +706,71 @@
       <c r="C11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="2"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="10"/>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1">
       <c r="A12" s="2"/>
       <c r="B12" s="1"/>
       <c r="C12" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="7">
         <v>2700.79</v>
       </c>
+      <c r="G12" s="10">
+        <v>9.9499999999999993</v>
+      </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
       <c r="A13" s="2"/>
       <c r="B13" s="1"/>
       <c r="C13" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="7">
         <v>3100.33</v>
       </c>
+      <c r="G13" s="10">
+        <v>46.05</v>
+      </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
       <c r="A14" s="2"/>
       <c r="B14" s="1"/>
       <c r="C14" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="7">
         <v>1850.42</v>
       </c>
+      <c r="G14" s="10">
+        <v>78</v>
+      </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
       <c r="A15" s="2"/>
       <c r="B15" t="s">
         <v>53</v>
@@ -715,74 +778,84 @@
       <c r="C15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="2"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="10"/>
     </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="7">
         <v>420.78</v>
       </c>
+      <c r="G16" s="10">
+        <v>30</v>
+      </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="7">
         <v>440.11</v>
       </c>
+      <c r="G17" s="10">
+        <v>65.5</v>
+      </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="7">
         <v>520.08000000000004</v>
       </c>
+      <c r="G18" s="10">
+        <v>40</v>
+      </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="20" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="22" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="23" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="24" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="25" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="28" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="29" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="30" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="31" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:7" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -1752,5 +1825,6 @@
     <row r="999" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated admin/Menu.xlsx (changed discounts numbers)
</commit_message>
<xml_diff>
--- a/admin/Menu.xlsx
+++ b/admin/Menu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dmitrii\PycharmProjects\FastAPI_Restaurant\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37A1692-C4AE-478C-9B3D-5A331E2480C2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149A0088-6697-4F7C-A39E-8403686072FB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,177 +16,172 @@
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjvwozj06heQVGmxYVZutM7iYW8Dw=="/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
+    <t>08f8c612-2700-406e-88df-eae964a98f67</t>
+  </si>
+  <si>
     <t>Меню</t>
   </si>
   <si>
     <t>Основное меню</t>
   </si>
   <si>
+    <t>c2ddea44-b60b-49ad-b919-7e40ecddcdb9</t>
+  </si>
+  <si>
     <t>Холодные закуски</t>
   </si>
   <si>
     <t>К пиву</t>
   </si>
   <si>
+    <t>2f14b53d-1bcc-4a1b-97ca-d08cfedbc31c</t>
+  </si>
+  <si>
     <t>Сельдь Бисмарк</t>
   </si>
   <si>
     <t>Традиционное немецкое блюдо из маринованной сельди</t>
   </si>
   <si>
+    <t>5b0a804a-d0c0-45c7-9ef0-bf5a5bba271a</t>
+  </si>
+  <si>
     <t>Мясная тарелка</t>
   </si>
   <si>
+    <t>Нарезка из ветчины, колбасных колечек, нескольких сортов сыра и фруктов</t>
+  </si>
+  <si>
+    <t>7580d708-5314-4212-a30d-81fad3738b59</t>
+  </si>
+  <si>
     <t>Рыбная тарелка</t>
   </si>
   <si>
     <t>Нарезка из креветок, кальмаров, раковых шеек, гребешков, лосося, скумбрии и красной икры</t>
   </si>
   <si>
+    <t>59c4f253-c906-4e42-a81d-75a735e299ef</t>
+  </si>
+  <si>
     <t>Рамен</t>
   </si>
   <si>
     <t>Горячий рамен</t>
   </si>
   <si>
+    <t>6e56c599-9fb4-47e6-b7cd-191e59634c7b</t>
+  </si>
+  <si>
     <t>Дайзу рамен</t>
   </si>
   <si>
     <t>Рамен на курином бульоне с куриными подушками и яйцом аджитама, яично-пшеничной лапшой, ростки зелени, грибами муэр и зеленым луком</t>
   </si>
   <si>
+    <t>ee3fad65-2876-45c4-9e91-7ca21405df92</t>
+  </si>
+  <si>
     <t>Унаги рамен</t>
   </si>
   <si>
     <t>Рамен на нежном сливочном рыбном бульоне, с добавлением маринованного угря, грибов муэр, кунжута, зеленого лука</t>
   </si>
   <si>
+    <t>230daedc-6335-416f-95b4-ecfd952f60dc</t>
+  </si>
+  <si>
     <t>Чиизу Рамен</t>
   </si>
   <si>
     <t>Рамен на насыщенном сырном бульоне на основе кокосового молока, с добавлением куриной грудинки, яично - пшеничной лапши, мисо-матадоре, ростков зелени, листьев вакамэ</t>
   </si>
   <si>
+    <t>7cbb7091-747e-4d5c-82e5-d7da589888e9</t>
+  </si>
+  <si>
     <t>Алкогольное меню</t>
   </si>
   <si>
     <t>Алкогольные напитки</t>
   </si>
   <si>
+    <t>2cc28716-4861-4ca0-b78e-aa9194c28e1f</t>
+  </si>
+  <si>
     <t>Красные вина</t>
   </si>
   <si>
     <t>Для романтичного вечера</t>
   </si>
   <si>
+    <t>29a5e408-08c7-4f66-9432-972dd4d644b3</t>
+  </si>
+  <si>
     <t>Шемен де Пап ля Ноблесс</t>
   </si>
   <si>
     <t>Вино красное — фруктовое, среднетелое, выдержанное в дубе</t>
   </si>
   <si>
+    <t>2cde7d42-04a6-42ad-8d2d-7ed704185105</t>
+  </si>
+  <si>
     <t>Рипароссо Монтепульчано</t>
   </si>
   <si>
     <t>Вино красное, сухое</t>
   </si>
   <si>
+    <t>f48aab6b-64e7-4aa8-8b0e-f70c4afe8cec</t>
+  </si>
+  <si>
     <t>Кьянти, Серристори</t>
   </si>
   <si>
     <t>Вино красное — элегантное, комплексное, не выдержанное в дубе</t>
   </si>
   <si>
+    <t>c27fa7a9-1170-4224-b73d-eb1b9e8c58a8</t>
+  </si>
+  <si>
     <t>Виски</t>
   </si>
   <si>
     <t>Для интересных бесед</t>
   </si>
   <si>
+    <t>b27a63ba-0104-4471-992a-a6503a940cd0</t>
+  </si>
+  <si>
     <t>Джемисон</t>
   </si>
   <si>
     <t>Классический купажированный виски, проходящий 4-хлетнюю выдержку в дубовых бочках</t>
   </si>
   <si>
+    <t>3117ee28-6d3f-4586-a027-7addd15d0c42</t>
+  </si>
+  <si>
     <t>Джек Дэниелс</t>
   </si>
   <si>
     <t>Характерен мягкий вкус, сочетает в себе карамельно-ванильные и древесные нотки. Легкий привкус дыма.</t>
   </si>
   <si>
+    <t>f1c96124-e005-467e-b2f6-86be90a8eb03</t>
+  </si>
+  <si>
     <t>Чивас Ригал</t>
   </si>
   <si>
     <t>Это купаж высококачественных солодовых и зерновых виски, выдержанных как минимум в течение 12 лет, что придает напитку роскошные нотки меда, ванили и спелых яблок.</t>
-  </si>
-  <si>
-    <t>Нарезка из ветчины, колбасных колечек, нескольких сортов сыра и фруктов</t>
-  </si>
-  <si>
-    <t>c2ddea44-b60b-49ad-b919-7e40ecddcdb9</t>
-  </si>
-  <si>
-    <t>08f8c612-2700-406e-88df-eae964a98f67</t>
-  </si>
-  <si>
-    <t>7cbb7091-747e-4d5c-82e5-d7da589888e9</t>
-  </si>
-  <si>
-    <t>59c4f253-c906-4e42-a81d-75a735e299ef</t>
-  </si>
-  <si>
-    <t>2f14b53d-1bcc-4a1b-97ca-d08cfedbc31c</t>
-  </si>
-  <si>
-    <t>5b0a804a-d0c0-45c7-9ef0-bf5a5bba271a</t>
-  </si>
-  <si>
-    <t>7580d708-5314-4212-a30d-81fad3738b59</t>
-  </si>
-  <si>
-    <t>29a5e408-08c7-4f66-9432-972dd4d644b3</t>
-  </si>
-  <si>
-    <t>2cde7d42-04a6-42ad-8d2d-7ed704185105</t>
-  </si>
-  <si>
-    <t>f48aab6b-64e7-4aa8-8b0e-f70c4afe8cec</t>
-  </si>
-  <si>
-    <t>b27a63ba-0104-4471-992a-a6503a940cd0</t>
-  </si>
-  <si>
-    <t>3117ee28-6d3f-4586-a027-7addd15d0c42</t>
-  </si>
-  <si>
-    <t>f1c96124-e005-467e-b2f6-86be90a8eb03</t>
-  </si>
-  <si>
-    <t>6e56c599-9fb4-47e6-b7cd-191e59634c7b</t>
-  </si>
-  <si>
-    <t>ee3fad65-2876-45c4-9e91-7ca21405df92</t>
-  </si>
-  <si>
-    <t>230daedc-6335-416f-95b4-ecfd952f60dc</t>
-  </si>
-  <si>
-    <t>2cc28716-4861-4ca0-b78e-aa9194c28e1f</t>
-  </si>
-  <si>
-    <t>c27fa7a9-1170-4224-b73d-eb1b9e8c58a8</t>
   </si>
 </sst>
 </file>
@@ -272,7 +267,12 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -283,13 +283,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -511,7 +506,7 @@
   <dimension ref="A1:G999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
@@ -519,327 +514,320 @@
     <col min="1" max="1" width="7.44140625" customWidth="1"/>
     <col min="2" max="2" width="20.88671875" customWidth="1"/>
     <col min="3" max="3" width="20.109375" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="77.6640625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="77.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="12.5546875" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="9"/>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A2" s="2"/>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="9"/>
+      <c r="C2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A3" s="2"/>
-      <c r="B3" s="1"/>
-      <c r="C3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="8">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="10">
         <v>182.99</v>
       </c>
-      <c r="G3" s="10">
-        <v>15</v>
+      <c r="G3" s="2">
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="16.5" customHeight="1">
-      <c r="A4" s="2"/>
-      <c r="B4" s="1"/>
-      <c r="C4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="8">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="10">
         <v>215.36</v>
       </c>
-      <c r="G4" s="10">
-        <v>25</v>
+      <c r="G4" s="2">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A5" s="2"/>
-      <c r="B5" s="1"/>
-      <c r="C5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="8">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="10">
         <v>265.57</v>
       </c>
-      <c r="G5" s="10">
-        <v>31</v>
+      <c r="G5" s="2">
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A6" s="2"/>
-      <c r="B6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="10"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="7">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="9">
         <v>166.47</v>
       </c>
-      <c r="G7" s="10">
-        <v>25.5</v>
-      </c>
+      <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="7">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="9">
         <v>168.25</v>
       </c>
-      <c r="G8" s="10">
-        <v>73</v>
-      </c>
+      <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="7">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="9">
         <v>132.88</v>
       </c>
-      <c r="G9" s="10">
-        <v>99.99</v>
-      </c>
+      <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="10"/>
+      <c r="A10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A11" s="2"/>
-      <c r="B11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="10"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A12" s="2"/>
-      <c r="B12" s="1"/>
-      <c r="C12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="7">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="9">
         <v>2700.79</v>
       </c>
-      <c r="G12" s="10">
-        <v>9.9499999999999993</v>
+      <c r="G12" s="2">
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A13" s="2"/>
-      <c r="B13" s="1"/>
-      <c r="C13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="7">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="9">
         <v>3100.33</v>
       </c>
-      <c r="G13" s="10">
-        <v>46.05</v>
+      <c r="G13" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A14" s="2"/>
-      <c r="B14" s="1"/>
-      <c r="C14" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="7">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="9">
         <v>1850.42</v>
       </c>
-      <c r="G14" s="10">
-        <v>78</v>
+      <c r="G14" s="2">
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A15" s="2"/>
-      <c r="B15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="10"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" t="s">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" s="7">
+      <c r="E16" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="9">
         <v>420.78</v>
       </c>
-      <c r="G16" s="10">
-        <v>30</v>
-      </c>
+      <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="7">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="9">
         <v>440.11</v>
       </c>
-      <c r="G17" s="10">
-        <v>65.5</v>
+      <c r="G17" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="7">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="9">
         <v>520.08000000000004</v>
       </c>
-      <c r="G18" s="10">
-        <v>40</v>
+      <c r="G18" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1"/>

</xml_diff>